<commit_message>
Alterações no Mapeamento dos resultados e nos passos em "Especificar os requisitos" e "Validar os requisitos".
</commit_message>
<xml_diff>
--- a/Doc de atividades.xlsx
+++ b/Doc de atividades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>Levantamento de requisitos</t>
   </si>
@@ -59,30 +59,15 @@
     <t>Artefato de saída: Ata da reunião. Documento que descreve as necessidades do cliente</t>
   </si>
   <si>
-    <t>O gerente do projeto cria a ata da reunião</t>
-  </si>
-  <si>
     <t>Critério de entrada: Solicitação do cliente</t>
   </si>
   <si>
     <t>Responsável: Gerente do projeto, Analista de desenvolvimento e Analista de requisito</t>
   </si>
   <si>
-    <t>O gerente do projeto e analista de requisitos validam o documento de requisitos com o cliente</t>
-  </si>
-  <si>
     <t>Responsável: Gerente do projeto, Analista requisitos e Analista de desenvolvimento</t>
   </si>
   <si>
-    <t>Analista de desenvolvimento prepara o diagrama de caso de uso</t>
-  </si>
-  <si>
-    <t>Analista de desenvolvimento prepara o diagrama de classe</t>
-  </si>
-  <si>
-    <t>Analista de desenvolvimento prepara o diagrama de sequência para principais funcionalidades</t>
-  </si>
-  <si>
     <t>O gerente do projeto e o analista de requisitos se reunem com o cliente</t>
   </si>
   <si>
@@ -110,9 +95,6 @@
     <t>GRE01</t>
   </si>
   <si>
-    <t xml:space="preserve">O gerente do projeto envia a ata para o cliente, por e-mai. O mesmo deve responder o e-mail confirmando o recebimento e dando o aval positivo. </t>
-  </si>
-  <si>
     <t>GRE02</t>
   </si>
   <si>
@@ -131,47 +113,90 @@
     <t>NÃO ATENDIDO</t>
   </si>
   <si>
-    <t>Existe a necessidade de criar um passo para identificar o modelo do documento de requisitos definido pela empresa.</t>
-  </si>
-  <si>
-    <t>Nenhum ponto</t>
-  </si>
-  <si>
-    <t>Existe a necessidade de criar um passo para o controle de mudança do documento de requistos e produtos do projeto (Os artefatos relacionados com o processo).</t>
-  </si>
-  <si>
-    <t>Passo 4 da atividade "Especificar os requisitos" e passo 1 da atividade "Validar os requisitos".</t>
-  </si>
-  <si>
     <t>Nenhuma atividade</t>
   </si>
   <si>
     <t>Existe a necessidade de criar uma atividade para controle de mudanças.</t>
   </si>
   <si>
-    <t>São os passo 1 e 2 da atividade "Levantamento de requisitos"</t>
-  </si>
-  <si>
     <t>É gerado o artefato de saída da atividade "Levantamento de requisitos", ata de reunião, onde comprova todos os requisitos solicitados pelo cliente.</t>
   </si>
   <si>
-    <t xml:space="preserve">Atendido nos passo 2 e </t>
-  </si>
-  <si>
-    <t>Gerente do projeto reune a equipe técnica (analista de desenvolvimento e analista de teste) para discutir a ata da reunião. O gerente de projetos envia um e-mail para todos os envolvidos, definindo o compromentimento com os requisitos</t>
-  </si>
-  <si>
-    <t>Analista de desenvolvimento prepara o documento de requisitos com base em um modelo definido pela empresa</t>
-  </si>
-  <si>
-    <t>Analista de requisito revisa o documento de requisitos</t>
+    <t>O gerente do projeto cria a ata da reunião.</t>
+  </si>
+  <si>
+    <t>O gerente do projeto envia a ata para o cliente, por e-mail. O mesmo deve responder o e-mail confirmando o recebimento e dando o aval positivo.</t>
+  </si>
+  <si>
+    <t>O gerente do projeto deve versionar a ata de reunião.</t>
+  </si>
+  <si>
+    <t>Analista de requisito revisa o documento de requisitos. O analista de requisito versiona a revisão do documento de requisitos.</t>
+  </si>
+  <si>
+    <t>Analista de desenvolvimento prepara o documento de requisitos com base em um modelo definido pela empresa. O analista de desenvolvimento versiona o documento de requisitos</t>
+  </si>
+  <si>
+    <t>Analista de desenvolvimento prepara o diagrama de caso de uso. O analista de desenvolvimento versiona o diagrama de caso de uso.</t>
+  </si>
+  <si>
+    <t>Analista de desenvolvimento prepara o diagrama de classe. O analista de desenvolvimento versiona o diagrama de classe.</t>
+  </si>
+  <si>
+    <t>Analista de desenvolvimento prepara o diagrama de sequência para principais funcionalidades. O analista de desenvolvimento versiona o diagrama de sequência.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O gerente do projeto e analista de requisitos validam o documento de requisitos com o cliente. </t>
+  </si>
+  <si>
+    <t>O gerente do projeto deve revisar os diagramas criados e criar uma tag no controle de versão com todos os documentos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerente do projeto reune a equipe técnica (analista de desenvolvimento e analista de teste) para discutir a ata da reunião. O gerente de projetos envia um e-mail para todos os envolvidos, definindo o compromentimento com os requisitos. Cada participante da equipe técnica deve responder o e-mail confirmando o comprometimento. </t>
+  </si>
+  <si>
+    <t>Atendido no passo 2 da atividade "Especificação de requisitos".</t>
+  </si>
+  <si>
+    <t>São os passo 1 e 2 da atividade "Levantamento de requisitos".</t>
+  </si>
+  <si>
+    <t>O comprometimento da equipe técnica fica formalizado por e-mail.</t>
+  </si>
+  <si>
+    <t>Passo 2 da atividade "Levantamento de requisitos". Passo 2,3,4 da atividade "Especificação de requisitos". Passo 1,2,3,4 da atividade "Validação de requisitos".</t>
+  </si>
+  <si>
+    <t>Passo 4 da atividade "Especificar os requisitos" e passos 1 e 5 da atividade "Validar os requisitos".</t>
+  </si>
+  <si>
+    <t>Para cada artefato gerado tem pelo menos um passo para revisão.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A ata de reunião ou e-mail de solicitação de mudança deve ser registrado no controle de versão definindo para cada um uma identificação (versão).
+Todos os outros documentos (documento de requisitos, e-mail de confirmação de validação e documentos de diagramas) tem uma referencia da identificação (versão) da ata de reunião ou e-mail de solicitação de mudança. </t>
+  </si>
+  <si>
+    <t>Modificar os requisitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artefato de saída: </t>
+  </si>
+  <si>
+    <t>Artefato de entrada: E-mail de solicitação de mudança.</t>
+  </si>
+  <si>
+    <t>Responsável: Analista de requisitos</t>
+  </si>
+  <si>
+    <t>Critério de entrada: Requisitos não validados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,7 +235,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,18 +282,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -611,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="220" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -625,126 +660,171 @@
     <col min="4" max="4" width="46.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="2.125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="7" max="7" width="2.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="39.75" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -754,8 +834,11 @@
       <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -765,31 +848,42 @@
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
+      <c r="H12" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -798,7 +892,7 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -812,7 +906,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -829,83 +923,86 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>